<commit_message>
Revert "Merge branch 'vignesh'"
This reverts commit ae709775eb5a6faee5de90cd6a53538734615c90, reversing
changes made to 305a2d18d7135f521406def2294383fdf9ea8aa3.
</commit_message>
<xml_diff>
--- a/backend/DSEC/scan/data/Compromise_Assessment.xlsx
+++ b/backend/DSEC/scan/data/Compromise_Assessment.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DES\DSEC360-\backend\DSEC\scan\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9763919-7E4E-42EC-BA6A-21E8A3AA10D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="19">
   <si>
     <t xml:space="preserve">ID Number </t>
   </si>
@@ -77,15 +71,13 @@
   </si>
   <si>
     <t>Poweshell History</t>
-  </si>
-  <si>
-    <t>Download Directory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -167,47 +159,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="11">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -218,10 +210,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -259,71 +251,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -351,7 +343,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -374,11 +366,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -387,13 +379,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -403,7 +395,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -412,7 +404,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -421,7 +413,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -429,10 +421,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -497,24 +489,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="9" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="47.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -525,7 +515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -536,7 +526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -547,7 +537,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -558,7 +548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -569,7 +559,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -580,7 +570,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -591,7 +581,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -602,7 +592,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -613,7 +603,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -624,7 +614,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -635,7 +625,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -646,7 +636,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -657,7 +647,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -668,7 +658,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -679,7 +669,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -690,7 +680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -701,7 +691,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -712,7 +702,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -723,7 +713,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -734,7 +724,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -745,7 +735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -756,7 +746,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="7">
         <v>22</v>
       </c>
@@ -767,7 +757,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="7">
         <v>23</v>
       </c>
@@ -778,7 +768,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="7">
         <v>24</v>
       </c>
@@ -789,7 +779,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -800,7 +790,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -809,17 +799,6 @@
       </c>
       <c r="C27" s="6" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="7">
-        <v>27</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor code and add all the missing code
</commit_message>
<xml_diff>
--- a/backend/DSEC/scan/data/Compromise_Assessment.xlsx
+++ b/backend/DSEC/scan/data/Compromise_Assessment.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DES\DSEC360-\backend\DSEC\scan\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D917F275-C2C3-4756-BC4C-9D5E2115BEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="20">
   <si>
     <t xml:space="preserve">ID Number </t>
   </si>
@@ -71,13 +77,15 @@
   </si>
   <si>
     <t>Poweshell History</t>
+  </si>
+  <si>
+    <t>Download Directory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -159,47 +167,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -210,10 +218,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -251,71 +259,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -343,7 +351,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -366,11 +374,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -379,13 +387,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -395,7 +403,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -404,7 +412,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -413,7 +421,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -421,10 +429,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -489,22 +497,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="9" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="47.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="11.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -526,7 +536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -537,7 +547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -548,7 +558,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -559,7 +569,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -570,7 +580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -581,7 +591,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -592,7 +602,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -603,7 +613,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -614,7 +624,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -625,7 +635,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -636,7 +646,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -647,7 +657,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -658,7 +668,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row r="15" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -669,7 +679,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -680,7 +690,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row r="17" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -691,7 +701,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row r="18" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -702,7 +712,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -713,7 +723,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -724,7 +734,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -735,7 +745,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -746,7 +756,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>22</v>
       </c>
@@ -757,7 +767,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>23</v>
       </c>
@@ -768,7 +778,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>24</v>
       </c>
@@ -779,7 +789,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -790,7 +800,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -799,6 +809,17 @@
       </c>
       <c r="C27" s="6" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="7">
+        <v>27</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor validate.py, refactor make.py
</commit_message>
<xml_diff>
--- a/backend/DSEC/scan/data/Compromise_Assessment.xlsx
+++ b/backend/DSEC/scan/data/Compromise_Assessment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DES\DSEC360-\backend\DSEC\scan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D917F275-C2C3-4756-BC4C-9D5E2115BEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC93D968-A8E7-4386-8B21-06C9300B3407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t xml:space="preserve">ID Number </t>
   </si>
@@ -40,12 +40,6 @@
     <t>Current Running Service Signed</t>
   </si>
   <si>
-    <t>Check the service "Everyone Write Permission"</t>
-  </si>
-  <si>
-    <t>SMB shares</t>
-  </si>
-  <si>
     <t>Startup files</t>
   </si>
   <si>
@@ -61,9 +55,6 @@
     <t>Third Party Application</t>
   </si>
   <si>
-    <t>Hotfix</t>
-  </si>
-  <si>
     <t>Auto Runs</t>
   </si>
   <si>
@@ -73,13 +64,16 @@
     <t>Check Malicious Files</t>
   </si>
   <si>
-    <t>Linux</t>
-  </si>
-  <si>
-    <t>Poweshell History</t>
-  </si>
-  <si>
-    <t>Download Directory</t>
+    <t>Visual Basic for Applications</t>
+  </si>
+  <si>
+    <t>Suspicious Directory</t>
+  </si>
+  <si>
+    <t>Check the service Everyone Permission</t>
+  </si>
+  <si>
+    <t>Living off the Land</t>
   </si>
 </sst>
 </file>
@@ -122,7 +116,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -132,47 +126,29 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -181,20 +157,11 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -501,24 +468,24 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -532,7 +499,7 @@
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -543,7 +510,7 @@
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -554,19 +521,19 @@
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>6</v>
+      <c r="C4" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>7</v>
+      <c r="B5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -576,8 +543,8 @@
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>8</v>
+      <c r="C6" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -587,8 +554,8 @@
       <c r="B7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>9</v>
+      <c r="C7" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -598,8 +565,8 @@
       <c r="B8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>10</v>
+      <c r="C8" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -609,8 +576,8 @@
       <c r="B9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>11</v>
+      <c r="C9" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -620,8 +587,8 @@
       <c r="B10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>12</v>
+      <c r="C10" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -631,8 +598,8 @@
       <c r="B11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>13</v>
+      <c r="C11" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -642,8 +609,8 @@
       <c r="B12" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>14</v>
+      <c r="C12" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -653,173 +620,30 @@
       <c r="B13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>16</v>
+      <c r="C14" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7">
-        <v>15</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7">
-        <v>16</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7">
-        <v>17</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7">
-        <v>18</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7">
-        <v>19</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7">
-        <v>20</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7">
-        <v>21</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7">
-        <v>22</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="7">
-        <v>23</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="6" t="s">
+      <c r="B15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7">
-        <v>24</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="7">
-        <v>25</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="7">
-        <v>26</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="7">
-        <v>27</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add validate.py, ioc controls
</commit_message>
<xml_diff>
--- a/backend/DSEC/scan/data/Compromise_Assessment.xlsx
+++ b/backend/DSEC/scan/data/Compromise_Assessment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DES\DSEC360-\backend\DSEC\scan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC93D968-A8E7-4386-8B21-06C9300B3407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B63A07F-4899-4CBE-819D-BFD5116D92D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t xml:space="preserve">ID Number </t>
   </si>
@@ -43,12 +43,6 @@
     <t>Startup files</t>
   </si>
   <si>
-    <t>Event Fies Check</t>
-  </si>
-  <si>
-    <t>schedule Task</t>
-  </si>
-  <si>
     <t>Defender and Realtime monitoring</t>
   </si>
   <si>
@@ -74,6 +68,18 @@
   </si>
   <si>
     <t>Living off the Land</t>
+  </si>
+  <si>
+    <t>Windows Events</t>
+  </si>
+  <si>
+    <t>Schedule Task</t>
+  </si>
+  <si>
+    <t>Configuration Files</t>
+  </si>
+  <si>
+    <t>List All User Accounts</t>
   </si>
 </sst>
 </file>
@@ -468,10 +474,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,7 +528,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -533,7 +539,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -544,7 +550,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -566,7 +572,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -577,7 +583,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -588,7 +594,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -599,7 +605,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -610,7 +616,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -621,7 +627,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -632,7 +638,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -643,7 +649,29 @@
         <v>3</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>